<commit_message>
Changed to readReferenceFile from GenerateReferenceDataList
</commit_message>
<xml_diff>
--- a/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
+++ b/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\ExampleTuningCorrectorGasMixture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13FD9AD-4074-4AA9-81E7-6261233DAF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108ED4D6-2D51-436F-BB63-342FF0E113C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>Sim /6/1.06</t>
+    <t>Sim /6.629</t>
   </si>
 </sst>
 </file>
@@ -302,7 +302,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sim /6/1.06</c:v>
+                  <c:v>Sim /6.629</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -381,40 +381,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.0705387849652199E-3</c:v>
+                  <c:v>2.8210035420245887E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3987976324011681E-2</c:v>
+                  <c:v>6.8494472607168811E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9016729536006446E-2</c:v>
+                  <c:v>1.0991857226291899E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8188364437867446E-2</c:v>
+                  <c:v>1.2421907188621181E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.5765684658542767E-4</c:v>
+                  <c:v>2.4894819433824258E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.408859309253882E-2</c:v>
+                  <c:v>8.8186933107289502E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6011765599895744E-2</c:v>
+                  <c:v>4.7038385748410023E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.40560031597838836</c:v>
+                  <c:v>0.33364466072034243</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38163271823222322</c:v>
+                  <c:v>0.33074811892993367</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0081705433191053</c:v>
+                  <c:v>1.0000656049496832</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18802897116068396</c:v>
+                  <c:v>0.21177667756100468</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2250281129040676</c:v>
+                  <c:v>0.28957705136023687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,7 +743,43 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.9096894138232722E-2"/>
+                  <c:y val="4.8008894721493146E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -797,40 +833,40 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.4701161787384972</c:v>
+                  <c:v>3.8233607739370483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57938363472237731</c:v>
+                  <c:v>3.5247891141993097</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6862064417298821</c:v>
+                  <c:v>3.8470035968597971</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89254941924898867</c:v>
+                  <c:v>3.4443756209116758</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67456156473011153</c:v>
+                  <c:v>5.1072014191880362</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60689324090936458</c:v>
+                  <c:v>2.6323951742422973</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76377249454424823</c:v>
+                  <c:v>1.8374051331362464</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85647125545964342</c:v>
+                  <c:v>1.4193886020803774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94731525802324912</c:v>
+                  <c:v>1.2180179411465826</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0081705433191053</c:v>
+                  <c:v>0.99993439935404382</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1647812372785731</c:v>
+                  <c:v>0.76225849459778261</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.458515546600438</c:v>
+                  <c:v>0.53279675844817298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2481,15 +2517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2512,7 +2548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>12</v>
       </c>
@@ -2525,18 +2561,18 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2">
-        <v>3.2248626672378801E-2</v>
+        <v>1.8700432480080999E-2</v>
       </c>
       <c r="I2">
-        <f>H2/6/1.06</f>
-        <v>5.0705387849652199E-3</v>
+        <f>H2/6.629</f>
+        <v>2.8210035420245887E-3</v>
       </c>
       <c r="K2" s="1">
-        <f>I2/F2</f>
-        <v>0.4701161787384972</v>
+        <f>F2/I2</f>
+        <v>3.8233607739370483</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>13</v>
       </c>
@@ -2549,18 +2585,18 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3">
-        <v>8.8963529420714296E-2</v>
+        <v>4.5404985891292202E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="1">H3/6/1.06</f>
-        <v>1.3987976324011681E-2</v>
+        <f t="shared" ref="I3:I13" si="1">H3/6.629</f>
+        <v>6.8494472607168811E-3</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K13" si="2">I3/F3</f>
-        <v>0.57938363472237731</v>
+        <f t="shared" ref="K3:K13" si="2">F3/I3</f>
+        <v>3.5247891141993097</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>14</v>
       </c>
@@ -2573,18 +2609,18 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4">
-        <v>0.18454639984900101</v>
+        <v>7.2865021553088993E-2</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>2.9016729536006446E-2</v>
+        <v>1.0991857226291899E-2</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>0.6862064417298821</v>
+        <v>3.8470035968597971</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>15</v>
       </c>
@@ -2597,18 +2633,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5">
-        <v>0.24287799782483699</v>
+        <v>8.2344822753369795E-2</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>3.8188364437867446E-2</v>
+        <v>1.2421907188621181E-2</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>0.89254941924898867</v>
+        <v>3.4443756209116758</v>
+      </c>
+      <c r="U5">
+        <v>1.8700432480080999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>16</v>
       </c>
@@ -2621,18 +2660,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6">
-        <v>5.4546975442833203E-3</v>
+        <v>1.6502775802682099E-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>8.5765684658542767E-4</v>
+        <v>2.4894819433824258E-4</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>0.67456156473011153</v>
+        <v>5.1072014191880362</v>
+      </c>
+      <c r="U6">
+        <v>4.5404985891292202E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>24</v>
       </c>
@@ -2645,18 +2687,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7">
-        <v>8.9603452068546904E-2</v>
+        <v>5.8459117956822203E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>1.408859309253882E-2</v>
+        <v>8.8186933107289502E-3</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>0.60689324090936458</v>
+        <v>2.6323951742422973</v>
+      </c>
+      <c r="U7">
+        <v>7.2865021553088993E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>25</v>
       </c>
@@ -2669,18 +2714,21 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8">
-        <v>0.41983482921533699</v>
+        <v>0.31181745912621001</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>6.6011765599895744E-2</v>
+        <v>4.7038385748410023E-2</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>0.76377249454424823</v>
+        <v>1.8374051331362464</v>
+      </c>
+      <c r="U8">
+        <v>8.2344822753369795E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>26</v>
       </c>
@@ -2693,18 +2741,21 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
-        <v>2.5796180096225498</v>
+        <v>2.2117304559151498</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>0.40560031597838836</v>
+        <v>0.33364466072034243</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>0.85647125545964342</v>
+        <v>1.4193886020803774</v>
+      </c>
+      <c r="U9">
+        <v>1.6502775802682099E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>27</v>
       </c>
@@ -2717,18 +2768,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10">
-        <v>2.42718408795694</v>
+        <v>2.1925292803865299</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>0.38163271823222322</v>
+        <v>0.33074811892993367</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>0.94731525802324912</v>
+        <v>1.2180179411465826</v>
+      </c>
+      <c r="U10">
+        <v>5.8459117956822203E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>28</v>
       </c>
@@ -2741,18 +2795,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11">
-        <v>6.41196465550951</v>
+        <v>6.6294348952114497</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>1.0081705433191053</v>
+        <v>1.0000656049496832</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>1.0081705433191053</v>
+        <v>0.99993439935404382</v>
+      </c>
+      <c r="U11">
+        <v>0.31181745912621001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>29</v>
       </c>
@@ -2765,18 +2822,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12">
-        <v>1.1958642565819499</v>
+        <v>1.4038675955519</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>0.18802897116068396</v>
+        <v>0.21177667756100468</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="2"/>
-        <v>1.1647812372785731</v>
+        <v>0.76225849459778261</v>
+      </c>
+      <c r="U12">
+        <v>2.2117304559151498</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>30</v>
       </c>
@@ -2789,15 +2849,33 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
-        <v>1.43117879806987</v>
+        <v>1.9196062734670101</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>0.2250281129040676</v>
+        <v>0.28957705136023687</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
-        <v>1.458515546600438</v>
+        <f>F13/I13</f>
+        <v>0.53279675844817298</v>
+      </c>
+      <c r="U13">
+        <v>2.1925292803865299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>6.6294348952114497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>1.4038675955519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>1.9196062734670101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Reverse Tuning Coefficients
</commit_message>
<xml_diff>
--- a/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
+++ b/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\ExampleTuningCorrectorGasMixture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108ED4D6-2D51-436F-BB63-342FF0E113C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF906E31-F8A3-4818-BABF-2DE0FDA02EF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Molecular Mass</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Sim /6.629</t>
+  </si>
+  <si>
+    <t>Fitted Ratio</t>
+  </si>
+  <si>
+    <t>Reverse Ratio</t>
+  </si>
+  <si>
+    <t>Fitted Reverse Ratio</t>
   </si>
 </sst>
 </file>
@@ -2520,7 +2529,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,6 +2556,15 @@
       <c r="K1" t="s">
         <v>5</v>
       </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2">
@@ -2571,6 +2589,18 @@
         <f>F2/I2</f>
         <v>3.8233607739370483</v>
       </c>
+      <c r="L2" s="1">
+        <f>1/K2</f>
+        <v>0.2615499972738029</v>
+      </c>
+      <c r="N2">
+        <f>(D2^2)*-0.014887522+0.420918*D2+0.9383</f>
+        <v>3.8455128320000007</v>
+      </c>
+      <c r="O2">
+        <f>0.0112817207083844*(D2^2) +D2*( -0.408181546694434) + 3.7160769331443</f>
+        <v>0.44246615481844609</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D3">
@@ -2592,8 +2622,20 @@
         <v>6.8494472607168811E-3</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K13" si="2">F3/I3</f>
+        <f t="shared" ref="K3:K12" si="2">F3/I3</f>
         <v>3.5247891141993097</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L13" si="3">1/K3</f>
+        <v>0.28370491612436782</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N13" si="4">(D3^2)*-0.014887522+0.420918*D3+0.9383</f>
+        <v>3.8942427820000001</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O13" si="5">0.0112817207083844*(D3^2) +D3*( -0.408181546694434) + 3.7160769331443</f>
+        <v>0.31632762583362117</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -2619,6 +2661,18 @@
         <f t="shared" si="2"/>
         <v>3.8470035968597971</v>
       </c>
+      <c r="L4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25994256954068679</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>3.9131976880000003</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>0.21275253826556639</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5">
@@ -2643,6 +2697,18 @@
         <f t="shared" si="2"/>
         <v>3.4443756209116758</v>
       </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.29032838170400088</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>3.9023775499999998</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>0.13174089211427953</v>
+      </c>
       <c r="U5">
         <v>1.8700432480080999E-2</v>
       </c>
@@ -2670,6 +2736,18 @@
         <f t="shared" si="2"/>
         <v>5.1072014191880362</v>
       </c>
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.19580195060311212</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>3.8617823680000001</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>7.3292687379762356E-2</v>
+      </c>
       <c r="U6">
         <v>4.5404985891292202E-2</v>
       </c>
@@ -2697,6 +2775,18 @@
         <f t="shared" si="2"/>
         <v>2.6323951742422973</v>
       </c>
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.37988217338524705</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>2.4651193280000019</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>0.41799094050729879</v>
+      </c>
       <c r="U7">
         <v>7.2865021553088993E-2</v>
       </c>
@@ -2724,6 +2814,18 @@
         <f t="shared" si="2"/>
         <v>1.8374051331362464</v>
       </c>
+      <c r="L8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.54424578551879366</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>2.1565487499999989</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>0.56261370852369952</v>
+      </c>
       <c r="U8">
         <v>8.2344822753369795E-2</v>
       </c>
@@ -2751,6 +2853,18 @@
         <f t="shared" si="2"/>
         <v>1.4193886020803774</v>
       </c>
+      <c r="L9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.70452869533707285</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>1.8182031280000004</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>0.72979991795686994</v>
+      </c>
       <c r="U9">
         <v>1.6502775802682099E-3</v>
       </c>
@@ -2778,6 +2892,18 @@
         <f t="shared" si="2"/>
         <v>1.2180179411465826</v>
       </c>
+      <c r="L10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.82100596897501266</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>1.450082462000001</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>0.91954956880681094</v>
+      </c>
       <c r="U10">
         <v>5.8459117956822203E-2</v>
       </c>
@@ -2805,6 +2931,18 @@
         <f t="shared" si="2"/>
         <v>0.99993439935404382</v>
       </c>
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000656049496832</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>1.0521867520000008</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>1.1318626610735172</v>
+      </c>
       <c r="U11">
         <v>0.31181745912621001</v>
       </c>
@@ -2832,6 +2970,18 @@
         <f t="shared" si="2"/>
         <v>0.76225849459778261</v>
       </c>
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3118909229442768</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>0.62451599800000157</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>1.3667391947569931</v>
+      </c>
       <c r="U12">
         <v>2.2117304559151498</v>
       </c>
@@ -2858,6 +3008,18 @@
       <c r="K13" s="1">
         <f>F13/I13</f>
         <v>0.53279675844817298</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8768882958533868</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>0.16707019999999961</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="5"/>
+        <v>1.6241791698572388</v>
       </c>
       <c r="U13">
         <v>2.1925292803865299</v>

</xml_diff>

<commit_message>
TuningCorrection is not propagating correctly as described in TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated
</commit_message>
<xml_diff>
--- a/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
+++ b/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\ExampleTuningCorrectorGasMixture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF906E31-F8A3-4818-BABF-2DE0FDA02EF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8020F62-730F-4676-B042-8D9ACF4246D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Savara, Aditya Ashi</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{83EDC36A-F74C-4262-8DA7-48FB1715C519}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Savara, Aditya Ashi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Deleted 17, 21, 22</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{A3A8B18B-E0A7-42E3-8521-0837720768C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Savara, Aditya Ashi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+When copying out of TuningCorrectorGasMixtureSimulatedHypotheticalReferenceData.csv
+need to ignore m2 and m31</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Molecular Mass</t>
   </si>
@@ -54,9 +113,6 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>Sim /6.629</t>
-  </si>
-  <si>
     <t>Fitted Ratio</t>
   </si>
   <si>
@@ -65,18 +121,77 @@
   <si>
     <t>Fitted Reverse Ratio</t>
   </si>
+  <si>
+    <t>Sim /100</t>
+  </si>
+  <si>
+    <t>Consider what should happen to Butanal m28 to m18.</t>
+  </si>
+  <si>
+    <t>In the original pattern from Literature, m28 to 18 is :</t>
+  </si>
+  <si>
+    <t>So a case where we have a measurement like this:</t>
+  </si>
+  <si>
+    <t>m28</t>
+  </si>
+  <si>
+    <t>m18</t>
+  </si>
+  <si>
+    <t>Should become like this:</t>
+  </si>
+  <si>
+    <t>Final ratio:</t>
+  </si>
+  <si>
+    <t>Currently, what is coming out is like this in the mixed pattern:</t>
+  </si>
+  <si>
+    <t>m23/m18 Ratio:</t>
+  </si>
+  <si>
+    <t>So the mixed pattern is not propagating the tuning correction properly for some reason.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,6 +362,9 @@
                 <c:pt idx="11">
                   <c:v>30</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -311,7 +429,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sim /6.629</c:v>
+                  <c:v>Sim /100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -380,6 +498,9 @@
                 <c:pt idx="11">
                   <c:v>30</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -387,43 +508,43 @@
             <c:numRef>
               <c:f>Sheet1!$I$2:$I$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2.8210035420245887E-3</c:v>
+                  <c:v>5.0294454827771E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8494472607168811E-3</c:v>
+                  <c:v>1.3874613195859E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0991857226291899E-2</c:v>
+                  <c:v>2.8781568483916803E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2421907188621181E-2</c:v>
+                  <c:v>3.7878873461372399E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4894819433824258E-4</c:v>
+                  <c:v>8.5070611541757904E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8186933107289502E-3</c:v>
+                  <c:v>1.39744145332358E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7038385748410023E-2</c:v>
+                  <c:v>6.5476784694156395E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33364466072034243</c:v>
+                  <c:v>0.40231319856169101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33074811892993367</c:v>
+                  <c:v>0.37853984205470803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0000656049496832</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21177667756100468</c:v>
+                  <c:v>0.186505122974188</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28957705136023687</c:v>
+                  <c:v>0.22320441159015497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -842,40 +963,40 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.8233607739370483</c:v>
+                  <c:v>2.1445136094324968</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5247891141993097</c:v>
+                  <c:v>1.7400742494257635</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8470035968597971</c:v>
+                  <c:v>1.4691942278734262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4443756209116758</c:v>
+                  <c:v>1.1295403050818213</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1072014191880362</c:v>
+                  <c:v>1.4945567551309726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6323951742422973</c:v>
+                  <c:v>1.6611991621598481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8374051331362464</c:v>
+                  <c:v>1.3199880206745236</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4193886020803774</c:v>
+                  <c:v>1.1771212832800235</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2180179411465826</c:v>
+                  <c:v>1.0642397393902869</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99993439935404382</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.76225849459778261</c:v>
+                  <c:v>0.86554497192504942</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.53279675844817298</c:v>
+                  <c:v>0.69123057732842541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2227,15 +2348,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2525,16 +2646,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2551,22 +2672,25 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
+      <c r="T1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>12</v>
       </c>
@@ -2578,20 +2702,20 @@
         <v>1.0785714285714286E-2</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2">
-        <v>1.8700432480080999E-2</v>
-      </c>
-      <c r="I2">
-        <f>H2/6.629</f>
-        <v>2.8210035420245887E-3</v>
+      <c r="H2" s="1">
+        <v>0.50294454827770996</v>
+      </c>
+      <c r="I2" s="1">
+        <f>H2/100</f>
+        <v>5.0294454827771E-3</v>
       </c>
       <c r="K2" s="1">
         <f>F2/I2</f>
-        <v>3.8233607739370483</v>
+        <v>2.1445136094324968</v>
       </c>
       <c r="L2" s="1">
         <f>1/K2</f>
-        <v>0.2615499972738029</v>
+        <v>0.46630620370118808</v>
       </c>
       <c r="N2">
         <f>(D2^2)*-0.014887522+0.420918*D2+0.9383</f>
@@ -2601,8 +2725,11 @@
         <f>0.0112817207083844*(D2^2) +D2*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.44246615481844609</v>
       </c>
+      <c r="T2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>13</v>
       </c>
@@ -2614,31 +2741,35 @@
         <v>2.4142857142857143E-2</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3">
-        <v>4.5404985891292202E-2</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I13" si="1">H3/6.629</f>
-        <v>6.8494472607168811E-3</v>
+      <c r="H3" s="1">
+        <v>1.3874613195859</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I13" si="1">H3/100</f>
+        <v>1.3874613195859E-2</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K12" si="2">F3/I3</f>
-        <v>3.5247891141993097</v>
+        <v>1.7400742494257635</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L13" si="3">1/K3</f>
-        <v>0.28370491612436782</v>
+        <v>0.57468812053853846</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N13" si="4">(D3^2)*-0.014887522+0.420918*D3+0.9383</f>
+        <f>(D3^2)*-0.014887522+0.420918*D3+0.9383</f>
         <v>3.8942427820000001</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O13" si="5">0.0112817207083844*(D3^2) +D3*( -0.408181546694434) + 3.7160769331443</f>
+        <f>0.0112817207083844*(D3^2) +D3*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.31632762583362117</v>
       </c>
+      <c r="T3">
+        <f>1491/150</f>
+        <v>9.94</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>14</v>
       </c>
@@ -2650,31 +2781,34 @@
         <v>4.2285714285714288E-2</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4">
-        <v>7.2865021553088993E-2</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="1">
+        <v>2.8781568483916802</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>1.0991857226291899E-2</v>
+        <v>2.8781568483916803E-2</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>3.8470035968597971</v>
+        <v>1.4691942278734262</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="3"/>
-        <v>0.25994256954068679</v>
+        <v>0.68064520063316758</v>
       </c>
       <c r="N4">
-        <f t="shared" si="4"/>
+        <f>(D4^2)*-0.014887522+0.420918*D4+0.9383</f>
         <v>3.9131976880000003</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D4^2) +D4*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.21275253826556639</v>
       </c>
+      <c r="T4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>15</v>
       </c>
@@ -2686,34 +2820,40 @@
         <v>4.2785714285714288E-2</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5">
-        <v>8.2344822753369795E-2</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="1">
+        <v>3.7878873461372402</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>1.2421907188621181E-2</v>
+        <v>3.7878873461372399E-2</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>3.4443756209116758</v>
+        <v>1.1295403050818213</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>0.29032838170400088</v>
+        <v>0.8853159072774851</v>
       </c>
       <c r="N5">
-        <f t="shared" si="4"/>
+        <f>(D5^2)*-0.014887522+0.420918*D5+0.9383</f>
         <v>3.9023775499999998</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D5^2) +D5*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.13174089211427953</v>
       </c>
-      <c r="U5">
-        <v>1.8700432480080999E-2</v>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>16</v>
       </c>
@@ -2725,34 +2865,41 @@
         <v>1.2714285714285716E-3</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6">
-        <v>1.6502775802682099E-3</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="1">
+        <v>8.5070611541757907E-2</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>2.4894819433824258E-4</v>
+        <v>8.5070611541757904E-4</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>5.1072014191880362</v>
+        <v>1.4945567551309726</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>0.19580195060311212</v>
+        <v>0.66909469751944406</v>
       </c>
       <c r="N6">
-        <f t="shared" si="4"/>
+        <f>(D6^2)*-0.014887522+0.420918*D6+0.9383</f>
         <v>3.8617823680000001</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D6^2) +D6*( -0.408181546694434) + 3.7160769331443</f>
         <v>7.3292687379762356E-2</v>
       </c>
+      <c r="T6">
+        <v>9.94</v>
+      </c>
       <c r="U6">
-        <v>4.5404985891292202E-2</v>
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <f>T6/U6</f>
+        <v>9.94</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>24</v>
       </c>
@@ -2764,34 +2911,34 @@
         <v>2.3214285714285715E-2</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7">
-        <v>5.8459117956822203E-2</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="1">
+        <v>1.3974414533235799</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>8.8186933107289502E-3</v>
+        <v>1.39744145332358E-2</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>2.6323951742422973</v>
+        <v>1.6611991621598481</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>0.37988217338524705</v>
+        <v>0.60197477989323445</v>
       </c>
       <c r="N7">
-        <f t="shared" si="4"/>
+        <f>(D7^2)*-0.014887522+0.420918*D7+0.9383</f>
         <v>2.4651193280000019</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D7^2) +D7*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.41799094050729879</v>
       </c>
-      <c r="U7">
-        <v>7.2865021553088993E-2</v>
+      <c r="T7" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>25</v>
       </c>
@@ -2803,34 +2950,40 @@
         <v>8.6428571428571438E-2</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8">
-        <v>0.31181745912621001</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="1">
+        <v>6.54767846941564</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>4.7038385748410023E-2</v>
+        <v>6.5476784694156395E-2</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>1.8374051331362464</v>
+        <v>1.3199880206745236</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>0.54424578551879366</v>
+        <v>0.75758263282494986</v>
       </c>
       <c r="N8">
-        <f t="shared" si="4"/>
+        <f>(D8^2)*-0.014887522+0.420918*D8+0.9383</f>
         <v>2.1565487499999989</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D8^2) +D8*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.56261370852369952</v>
       </c>
-      <c r="U8">
-        <v>8.2344822753369795E-2</v>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>26</v>
       </c>
@@ -2842,34 +2995,43 @@
         <v>0.47357142857142864</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9">
-        <v>2.2117304559151498</v>
-      </c>
-      <c r="I9">
+      <c r="H9" s="1">
+        <v>40.231319856169101</v>
+      </c>
+      <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>0.33364466072034243</v>
+        <v>0.40231319856169101</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>1.4193886020803774</v>
+        <v>1.1771212832800235</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>0.70452869533707285</v>
+        <v>0.84953013270945299</v>
       </c>
       <c r="N9">
-        <f t="shared" si="4"/>
+        <f>(D9^2)*-0.014887522+0.420918*D9+0.9383</f>
         <v>1.8182031280000004</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D9^2) +D9*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.72979991795686994</v>
       </c>
+      <c r="T9">
+        <f>N11*T6</f>
+        <v>10.458736314880007</v>
+      </c>
       <c r="U9">
-        <v>1.6502775802682099E-3</v>
+        <f>U6*N14</f>
+        <v>3.6912668719999999</v>
+      </c>
+      <c r="V9">
+        <f>T9/U9</f>
+        <v>2.8333731148550796</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>27</v>
       </c>
@@ -2881,34 +3043,34 @@
         <v>0.40285714285714286</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10">
-        <v>2.1925292803865299</v>
-      </c>
-      <c r="I10">
+      <c r="H10" s="1">
+        <v>37.853984205470802</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>0.33074811892993367</v>
+        <v>0.37853984205470803</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>1.2180179411465826</v>
+        <v>1.0642397393902869</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>0.82100596897501266</v>
+        <v>0.93963790580955897</v>
       </c>
       <c r="N10">
-        <f t="shared" si="4"/>
+        <f>(D10^2)*-0.014887522+0.420918*D10+0.9383</f>
         <v>1.450082462000001</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D10^2) +D10*( -0.408181546694434) + 3.7160769331443</f>
         <v>0.91954956880681094</v>
       </c>
-      <c r="U10">
-        <v>5.8459117956822203E-2</v>
+      <c r="T10" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>28</v>
       </c>
@@ -2920,34 +3082,35 @@
         <v>1</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11">
-        <v>6.6294348952114497</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="1">
+        <v>100</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>1.0000656049496832</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>0.99993439935404382</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="3"/>
-        <v>1.0000656049496832</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <f t="shared" si="4"/>
+        <f>(D11^2)*-0.014887522+0.420918*D11+0.9383</f>
         <v>1.0521867520000008</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D11^2) +D11*( -0.408181546694434) + 3.7160769331443</f>
         <v>1.1318626610735172</v>
       </c>
-      <c r="U11">
-        <v>0.31181745912621001</v>
+      <c r="T11">
+        <f>T9/U9</f>
+        <v>2.8333731148550796</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>29</v>
       </c>
@@ -2959,34 +3122,34 @@
         <v>0.16142857142857145</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12">
-        <v>1.4038675955519</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="1">
+        <v>18.6505122974188</v>
+      </c>
+      <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>0.21177667756100468</v>
+        <v>0.186505122974188</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="2"/>
-        <v>0.76225849459778261</v>
+        <v>0.86554497192504942</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="3"/>
-        <v>1.3118909229442768</v>
+        <v>1.1553414697516069</v>
       </c>
       <c r="N12">
-        <f t="shared" si="4"/>
+        <f>(D12^2)*-0.014887522+0.420918*D12+0.9383</f>
         <v>0.62451599800000157</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D12^2) +D12*( -0.408181546694434) + 3.7160769331443</f>
         <v>1.3667391947569931</v>
       </c>
-      <c r="U12">
-        <v>2.2117304559151498</v>
+      <c r="T12" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>30</v>
       </c>
@@ -2998,50 +3161,70 @@
         <v>0.1542857142857143</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13">
-        <v>1.9196062734670101</v>
-      </c>
-      <c r="I13">
+      <c r="H13" s="1">
+        <v>22.320441159015498</v>
+      </c>
+      <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>0.28957705136023687</v>
+        <v>0.22320441159015497</v>
       </c>
       <c r="K13" s="1">
         <f>F13/I13</f>
-        <v>0.53279675844817298</v>
+        <v>0.69123057732842541</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="3"/>
-        <v>1.8768882958533868</v>
+        <v>1.4466952603065597</v>
       </c>
       <c r="N13">
-        <f t="shared" si="4"/>
+        <f>(D13^2)*-0.014887522+0.420918*D13+0.9383</f>
         <v>0.16707019999999961</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f>0.0112817207083844*(D13^2) +D13*( -0.408181546694434) + 3.7160769331443</f>
         <v>1.6241791698572388</v>
       </c>
-      <c r="U13">
-        <v>2.1925292803865299</v>
+      <c r="T13" t="s">
+        <v>13</v>
+      </c>
+      <c r="U13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="N14">
+        <f>(D14^2)*-0.014887522+0.420918*D14+0.9383</f>
+        <v>3.6912668719999999</v>
+      </c>
+      <c r="O14">
+        <f>0.0112817207083844*(D14^2) +D14*( -0.408181546694434) + 3.7160769331443</f>
+        <v>2.4086602161033532E-2</v>
+      </c>
+      <c r="T14">
+        <v>23</v>
+      </c>
       <c r="U14">
-        <v>6.6294348952114497</v>
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <f>T14/U14</f>
+        <v>7.666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U15">
-        <v>1.4038675955519</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U16">
-        <v>1.9196062734670101</v>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing TuningCorrectorGaxMixture rounding problem. It was in XYYYDataFunctions
</commit_message>
<xml_diff>
--- a/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
+++ b/ExampleTuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\ExampleTuningCorrectorGasMixture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8020F62-730F-4676-B042-8D9ACF4246D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5270E44C-D4FB-4B45-9261-0883841DED09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Savara, Aditya Ashi:</t>
         </r>
@@ -56,7 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Deleted 17, 21, 22</t>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Molecular Mass</t>
   </si>
@@ -146,20 +146,26 @@
     <t>Final ratio:</t>
   </si>
   <si>
-    <t>Currently, what is coming out is like this in the mixed pattern:</t>
-  </si>
-  <si>
     <t>m23/m18 Ratio:</t>
   </si>
   <si>
-    <t>So the mixed pattern is not propagating the tuning correction properly for some reason.</t>
+    <t>Currently, what is coming out is like this in the mixed pattern, before standardizing:</t>
+  </si>
+  <si>
+    <t>This looks good!</t>
+  </si>
+  <si>
+    <t>And after standardizin we are getting:</t>
+  </si>
+  <si>
+    <t>So the Mixed Reference Pattern coming out is as expected.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,19 +185,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2647,15 +2640,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2690,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>12</v>
       </c>
@@ -2718,18 +2711,18 @@
         <v>0.46630620370118808</v>
       </c>
       <c r="N2">
-        <f>(D2^2)*-0.014887522+0.420918*D2+0.9383</f>
-        <v>3.8455128320000007</v>
+        <f>(D2^2)*-0.00209891515351478+0.0415721558521753*D2+1.48645618255443</f>
+        <v>1.6830782706744052</v>
       </c>
       <c r="O2">
-        <f>0.0112817207083844*(D2^2) +D2*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.44246615481844609</v>
+        <f>0.00453957499583183*(D2^2) +D2*(-0.158786664417733) + 1.94715165380596</f>
+        <v>0.69541048019294749</v>
       </c>
       <c r="T2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>13</v>
       </c>
@@ -2757,19 +2750,19 @@
         <v>0.57468812053853846</v>
       </c>
       <c r="N3">
-        <f>(D3^2)*-0.014887522+0.420918*D3+0.9383</f>
-        <v>3.8942427820000001</v>
+        <f t="shared" ref="N3:N14" si="4">(D3^2)*-0.00209891515351478+0.0415721558521753*D3+1.48645618255443</f>
+        <v>1.6721775476887111</v>
       </c>
       <c r="O3">
-        <f>0.0112817207083844*(D3^2) +D3*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.31632762583362117</v>
+        <f t="shared" ref="O3:O14" si="5">0.00453957499583183*(D3^2) +D3*(-0.158786664417733) + 1.94715165380596</f>
+        <v>0.65011319067101025</v>
       </c>
       <c r="T3">
         <f>1491/150</f>
         <v>9.94</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>14</v>
       </c>
@@ -2797,18 +2790,18 @@
         <v>0.68064520063316758</v>
       </c>
       <c r="N4">
-        <f>(D4^2)*-0.014887522+0.420918*D4+0.9383</f>
-        <v>3.9131976880000003</v>
+        <f t="shared" si="4"/>
+        <v>1.6570789943959872</v>
       </c>
       <c r="O4">
-        <f>0.0112817207083844*(D4^2) +D4*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.21275253826556639</v>
+        <f t="shared" si="5"/>
+        <v>0.61389505114073639</v>
       </c>
       <c r="T4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>15</v>
       </c>
@@ -2836,12 +2829,12 @@
         <v>0.8853159072774851</v>
       </c>
       <c r="N5">
-        <f>(D5^2)*-0.014887522+0.420918*D5+0.9383</f>
-        <v>3.9023775499999998</v>
+        <f t="shared" si="4"/>
+        <v>1.6377826107962341</v>
       </c>
       <c r="O5">
-        <f>0.0112817207083844*(D5^2) +D5*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.13174089211427953</v>
+        <f t="shared" si="5"/>
+        <v>0.58675606160212657</v>
       </c>
       <c r="T5" t="s">
         <v>13</v>
@@ -2850,10 +2843,10 @@
         <v>14</v>
       </c>
       <c r="V5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>16</v>
       </c>
@@ -2881,12 +2874,12 @@
         <v>0.66909469751944406</v>
       </c>
       <c r="N6">
-        <f>(D6^2)*-0.014887522+0.420918*D6+0.9383</f>
-        <v>3.8617823680000001</v>
+        <f t="shared" si="4"/>
+        <v>1.6142883968894512</v>
       </c>
       <c r="O6">
-        <f>0.0112817207083844*(D6^2) +D6*( -0.408181546694434) + 3.7160769331443</f>
-        <v>7.3292687379762356E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.56869622205518033</v>
       </c>
       <c r="T6">
         <v>9.94</v>
@@ -2899,7 +2892,7 @@
         <v>9.94</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>24</v>
       </c>
@@ -2927,18 +2920,18 @@
         <v>0.60197477989323445</v>
       </c>
       <c r="N7">
-        <f>(D7^2)*-0.014887522+0.420918*D7+0.9383</f>
-        <v>2.4651193280000019</v>
+        <f t="shared" si="4"/>
+        <v>1.2752127945821239</v>
       </c>
       <c r="O7">
-        <f>0.0112817207083844*(D7^2) +D7*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.41799094050729879</v>
+        <f t="shared" si="5"/>
+        <v>0.75106690537950227</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>25</v>
       </c>
@@ -2966,12 +2959,12 @@
         <v>0.75758263282494986</v>
       </c>
       <c r="N8">
-        <f>(D8^2)*-0.014887522+0.420918*D8+0.9383</f>
-        <v>2.1565487499999989</v>
+        <f t="shared" si="4"/>
+        <v>1.213938107912075</v>
       </c>
       <c r="O8">
-        <f>0.0112817207083844*(D8^2) +D8*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.56261370852369952</v>
+        <f t="shared" si="5"/>
+        <v>0.8147194157575286</v>
       </c>
       <c r="T8" t="s">
         <v>13</v>
@@ -2980,10 +2973,10 @@
         <v>14</v>
       </c>
       <c r="V8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>26</v>
       </c>
@@ -3011,27 +3004,27 @@
         <v>0.84953013270945299</v>
       </c>
       <c r="N9">
-        <f>(D9^2)*-0.014887522+0.420918*D9+0.9383</f>
-        <v>1.8182031280000004</v>
+        <f t="shared" si="4"/>
+        <v>1.1484655909349966</v>
       </c>
       <c r="O9">
-        <f>0.0112817207083844*(D9^2) +D9*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.72979991795686994</v>
+        <f t="shared" si="5"/>
+        <v>0.88745107612721918</v>
       </c>
       <c r="T9">
         <f>N11*T6</f>
-        <v>10.458736314880007</v>
+        <v>9.9889750366339207</v>
       </c>
       <c r="U9">
         <f>U6*N14</f>
-        <v>3.6912668719999999</v>
+        <v>1.5547064781547968</v>
       </c>
       <c r="V9">
         <f>T9/U9</f>
-        <v>2.8333731148550796</v>
+        <v>6.4249909400836449</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>27</v>
       </c>
@@ -3059,18 +3052,18 @@
         <v>0.93963790580955897</v>
       </c>
       <c r="N10">
-        <f>(D10^2)*-0.014887522+0.420918*D10+0.9383</f>
-        <v>1.450082462000001</v>
+        <f t="shared" si="4"/>
+        <v>1.0787952436508885</v>
       </c>
       <c r="O10">
-        <f>0.0112817207083844*(D10^2) +D10*( -0.408181546694434) + 3.7160769331443</f>
-        <v>0.91954956880681094</v>
+        <f t="shared" si="5"/>
+        <v>0.96926188648857314</v>
       </c>
       <c r="T10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>28</v>
       </c>
@@ -3098,19 +3091,19 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <f>(D11^2)*-0.014887522+0.420918*D11+0.9383</f>
-        <v>1.0521867520000008</v>
+        <f t="shared" si="4"/>
+        <v>1.0049270660597507</v>
       </c>
       <c r="O11">
-        <f>0.0112817207083844*(D11^2) +D11*( -0.408181546694434) + 3.7160769331443</f>
-        <v>1.1318626610735172</v>
+        <f t="shared" si="5"/>
+        <v>1.0601518468415905</v>
       </c>
       <c r="T11">
         <f>T9/U9</f>
-        <v>2.8333731148550796</v>
+        <v>6.4249909400836449</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>29</v>
       </c>
@@ -3138,18 +3131,18 @@
         <v>1.1553414697516069</v>
       </c>
       <c r="N12">
-        <f>(D12^2)*-0.014887522+0.420918*D12+0.9383</f>
-        <v>0.62451599800000157</v>
+        <f t="shared" si="4"/>
+        <v>0.92686105816158371</v>
       </c>
       <c r="O12">
-        <f>0.0112817207083844*(D12^2) +D12*( -0.408181546694434) + 3.7160769331443</f>
-        <v>1.3667391947569931</v>
+        <f t="shared" si="5"/>
+        <v>1.1601209571862721</v>
       </c>
       <c r="T12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>30</v>
       </c>
@@ -3177,12 +3170,12 @@
         <v>1.4466952603065597</v>
       </c>
       <c r="N13">
-        <f>(D13^2)*-0.014887522+0.420918*D13+0.9383</f>
-        <v>0.16707019999999961</v>
+        <f t="shared" si="4"/>
+        <v>0.84459721995638692</v>
       </c>
       <c r="O13">
-        <f>0.0112817207083844*(D13^2) +D13*( -0.408181546694434) + 3.7160769331443</f>
-        <v>1.6241791698572388</v>
+        <f t="shared" si="5"/>
+        <v>1.269169217522617</v>
       </c>
       <c r="T13" t="s">
         <v>13</v>
@@ -3191,35 +3184,66 @@
         <v>14</v>
       </c>
       <c r="V13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>18</v>
       </c>
       <c r="N14">
-        <f>(D14^2)*-0.014887522+0.420918*D14+0.9383</f>
-        <v>3.6912668719999999</v>
+        <f t="shared" si="4"/>
+        <v>1.5547064781547968</v>
       </c>
       <c r="O14">
-        <f>0.0112817207083844*(D14^2) +D14*( -0.408181546694434) + 3.7160769331443</f>
-        <v>2.4086602161033532E-2</v>
-      </c>
-      <c r="T14">
-        <v>23</v>
-      </c>
-      <c r="U14">
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0.55981399293627887</v>
+      </c>
+      <c r="T14" s="1">
+        <v>14.9849611</v>
+      </c>
+      <c r="U14" s="1">
+        <v>2.3322929499999998</v>
       </c>
       <c r="V14">
         <f>T14/U14</f>
-        <v>7.666666666666667</v>
+        <v>6.4249909515011829</v>
+      </c>
+      <c r="W14" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T15" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" t="s">
+        <v>14</v>
+      </c>
+      <c r="V16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="20:22" x14ac:dyDescent="0.25">
+      <c r="T17" s="1">
+        <v>23.56</v>
+      </c>
+      <c r="U17" s="1">
+        <v>3.6669999999999998</v>
+      </c>
+      <c r="V17">
+        <f>T17/U17</f>
+        <v>6.4248704663212433</v>
+      </c>
+    </row>
+    <row r="18" spans="20:22" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>